<commit_message>
Tried fixing badlift text size but to  no avail
</commit_message>
<xml_diff>
--- a/Steelmeet/Steelmeet/Testxlsx/Test invägning.xlsx
+++ b/Steelmeet/Steelmeet/Testxlsx/Test invägning.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="102">
   <si>
     <t xml:space="preserve">Grupp</t>
   </si>
@@ -172,103 +172,160 @@
     <t xml:space="preserve">Johannes Jonsson</t>
   </si>
   <si>
+    <t xml:space="preserve">980724lw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gusselby KK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tomas Vikenhag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">980725lw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fredrik Antonsson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">980726lw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Johan Bjur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">980727lw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liam Andersson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">980728lw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elis Mild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">980729lw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roberd Palm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">980730lw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mio Gustafsson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">980731lw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leo Richter Palm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">980732lw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tage Juthnäs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">980733lw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tommy Johansson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">800224tj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emil Johansson Findahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">020712ej</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simon Nilsson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">050302sn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mattias Svensson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">980512ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ostboll Ätaren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">980532ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rulle rull KK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gandalf Svensson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">180512ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajay Ghale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">280512ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pol Pot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">380512ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ben Dover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">340512ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sven Svensson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">982512ms</t>
+  </si>
+  <si>
     <t xml:space="preserve">Herr Senior Klassiskt Bänkpress</t>
   </si>
   <si>
-    <t xml:space="preserve">000000aa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gusselby KK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tomas Vikenhag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fredrik Antonsson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Johan Bjur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liam Andersson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elis Mild</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roberd Palm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mio Gustafsson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leo Richter Palm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tage Juthnäs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tommy Johansson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">800224tj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emil Johansson Findahl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">020712ej</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simon Nilsson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">050302sn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mattias Svensson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">980512ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ostboll Ätaren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">980532ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rulle rull KK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gandalf Svensson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">180512ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajay Ghale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">280512ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pol Pot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">380512ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ben Dover</t>
-  </si>
-  <si>
-    <t xml:space="preserve">340512ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sven Svensson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">982512ms</t>
+    <t xml:space="preserve">982513ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">982514ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">982515ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">982516ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">982517ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">982518ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">982519ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">982520ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">982521ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">982522ms</t>
   </si>
 </sst>
 </file>
@@ -398,8 +455,8 @@
   </sheetPr>
   <dimension ref="A1:P999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q7" activeCellId="0" sqref="Q7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R37" activeCellId="0" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -408,7 +465,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.63"/>
@@ -495,7 +552,7 @@
       </c>
       <c r="H2" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="I2" s="2" t="n">
         <v>10</v>
@@ -504,8 +561,7 @@
         <v>20</v>
       </c>
       <c r="K2" s="2" t="n">
-        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>227.5</v>
+        <v>0</v>
       </c>
       <c r="L2" s="2" t="n">
         <v>10</v>
@@ -518,11 +574,10 @@
       </c>
       <c r="O2" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>255</v>
+        <v>320</v>
       </c>
       <c r="P2" s="2" t="n">
-        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -549,7 +604,7 @@
       </c>
       <c r="H3" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>93</v>
+        <v>214</v>
       </c>
       <c r="I3" s="2" t="n">
         <v>10</v>
@@ -558,8 +613,7 @@
         <v>20</v>
       </c>
       <c r="K3" s="2" t="n">
-        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>157.5</v>
+        <v>0</v>
       </c>
       <c r="L3" s="2" t="n">
         <v>10</v>
@@ -572,11 +626,10 @@
       </c>
       <c r="O3" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>355</v>
+        <v>310</v>
       </c>
       <c r="P3" s="2" t="n">
-        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>147.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -603,7 +656,7 @@
       </c>
       <c r="H4" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>10</v>
@@ -612,8 +665,7 @@
         <v>20</v>
       </c>
       <c r="K4" s="2" t="n">
-        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>482.5</v>
+        <v>0</v>
       </c>
       <c r="L4" s="2" t="n">
         <v>10</v>
@@ -626,11 +678,10 @@
       </c>
       <c r="O4" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>367.5</v>
+        <v>227.5</v>
       </c>
       <c r="P4" s="2" t="n">
-        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>27.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -657,7 +708,7 @@
       </c>
       <c r="H5" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>282</v>
+        <v>73</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>10</v>
@@ -667,7 +718,7 @@
       </c>
       <c r="K5" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>57.5</v>
+        <v>95</v>
       </c>
       <c r="L5" s="2" t="n">
         <v>10</v>
@@ -680,11 +731,11 @@
       </c>
       <c r="O5" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>217.5</v>
+        <v>212.5</v>
       </c>
       <c r="P5" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>250</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -711,7 +762,7 @@
       </c>
       <c r="H6" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>250</v>
+        <v>102</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>10</v>
@@ -721,7 +772,7 @@
       </c>
       <c r="K6" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>112.5</v>
+        <v>275</v>
       </c>
       <c r="L6" s="2" t="n">
         <v>10</v>
@@ -734,11 +785,11 @@
       </c>
       <c r="O6" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>295</v>
+        <v>457.5</v>
       </c>
       <c r="P6" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>315</v>
+        <v>227.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -765,7 +816,7 @@
       </c>
       <c r="H7" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>176</v>
+        <v>283</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>10</v>
@@ -775,7 +826,7 @@
       </c>
       <c r="K7" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>487.5</v>
+        <v>365</v>
       </c>
       <c r="L7" s="2" t="n">
         <v>10</v>
@@ -788,11 +839,11 @@
       </c>
       <c r="O7" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>147.5</v>
+        <v>470</v>
       </c>
       <c r="P7" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>135</v>
+        <v>490</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -819,7 +870,7 @@
       </c>
       <c r="H8" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>123</v>
+        <v>159</v>
       </c>
       <c r="I8" s="2" t="n">
         <v>10</v>
@@ -829,7 +880,7 @@
       </c>
       <c r="K8" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>247.5</v>
+        <v>245</v>
       </c>
       <c r="L8" s="2" t="n">
         <v>10</v>
@@ -842,11 +893,11 @@
       </c>
       <c r="O8" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>487.5</v>
+        <v>470</v>
       </c>
       <c r="P8" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>302.5</v>
+        <v>422.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -873,7 +924,7 @@
       </c>
       <c r="H9" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>72</v>
+        <v>223</v>
       </c>
       <c r="I9" s="2" t="n">
         <v>10</v>
@@ -883,7 +934,7 @@
       </c>
       <c r="K9" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>280</v>
+        <v>397.5</v>
       </c>
       <c r="L9" s="2" t="n">
         <v>10</v>
@@ -896,11 +947,11 @@
       </c>
       <c r="O9" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>255</v>
+        <v>180</v>
       </c>
       <c r="P9" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>187.5</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -927,7 +978,7 @@
       </c>
       <c r="H10" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>185</v>
+        <v>82</v>
       </c>
       <c r="I10" s="2" t="n">
         <v>10</v>
@@ -937,7 +988,7 @@
       </c>
       <c r="K10" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>175</v>
+        <v>137.5</v>
       </c>
       <c r="L10" s="2" t="n">
         <v>10</v>
@@ -950,11 +1001,11 @@
       </c>
       <c r="O10" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>65</v>
+        <v>447.5</v>
       </c>
       <c r="P10" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>347.5</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -981,7 +1032,7 @@
       </c>
       <c r="H11" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>62</v>
+        <v>217</v>
       </c>
       <c r="I11" s="2" t="n">
         <v>10</v>
@@ -991,7 +1042,7 @@
       </c>
       <c r="K11" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>27.5</v>
+        <v>202.5</v>
       </c>
       <c r="L11" s="2" t="n">
         <v>10</v>
@@ -1004,11 +1055,11 @@
       </c>
       <c r="O11" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>482.5</v>
+        <v>375</v>
       </c>
       <c r="P11" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>462.5</v>
+        <v>312.5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1035,7 +1086,7 @@
       </c>
       <c r="H12" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="I12" s="2" t="n">
         <v>10</v>
@@ -1045,7 +1096,7 @@
       </c>
       <c r="K12" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>87.5</v>
+        <v>327.5</v>
       </c>
       <c r="L12" s="2" t="n">
         <v>10</v>
@@ -1058,11 +1109,11 @@
       </c>
       <c r="O12" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>207.5</v>
+        <v>445</v>
       </c>
       <c r="P12" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>377.5</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1089,7 +1140,7 @@
       </c>
       <c r="H13" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>119</v>
+        <v>197</v>
       </c>
       <c r="I13" s="2" t="n">
         <v>10</v>
@@ -1099,7 +1150,7 @@
       </c>
       <c r="K13" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>117.5</v>
+        <v>212.5</v>
       </c>
       <c r="L13" s="2" t="n">
         <v>10</v>
@@ -1112,11 +1163,11 @@
       </c>
       <c r="O13" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>242.5</v>
+        <v>347.5</v>
       </c>
       <c r="P13" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>412.5</v>
+        <v>427.5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1143,7 +1194,7 @@
       </c>
       <c r="H14" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>177</v>
+        <v>223</v>
       </c>
       <c r="I14" s="2" t="n">
         <v>10</v>
@@ -1153,7 +1204,7 @@
       </c>
       <c r="K14" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>160</v>
+        <v>317.5</v>
       </c>
       <c r="L14" s="2" t="n">
         <v>10</v>
@@ -1166,11 +1217,11 @@
       </c>
       <c r="O14" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>377.5</v>
+        <v>472.5</v>
       </c>
       <c r="P14" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>495</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1186,18 +1237,18 @@
       <c r="D15" s="4" t="n">
         <v>-83</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H15" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>285</v>
+        <v>132</v>
       </c>
       <c r="I15" s="2" t="n">
         <v>0</v>
@@ -1206,7 +1257,8 @@
         <v>20</v>
       </c>
       <c r="K15" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>215</v>
       </c>
       <c r="L15" s="2" t="n">
         <v>10</v>
@@ -1219,10 +1271,11 @@
       </c>
       <c r="O15" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>447.5</v>
+        <v>65</v>
       </c>
       <c r="P15" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>477.5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1230,7 +1283,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>11</v>
@@ -1238,18 +1291,18 @@
       <c r="D16" s="4" t="n">
         <v>-83</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H16" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>179</v>
+        <v>242</v>
       </c>
       <c r="I16" s="2" t="n">
         <v>0</v>
@@ -1258,7 +1311,8 @@
         <v>20</v>
       </c>
       <c r="K16" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>457.5</v>
       </c>
       <c r="L16" s="2" t="n">
         <v>10</v>
@@ -1271,10 +1325,11 @@
       </c>
       <c r="O16" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>97.5</v>
+        <v>327.5</v>
       </c>
       <c r="P16" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>395</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1290,18 +1345,18 @@
       <c r="D17" s="4" t="n">
         <v>-83</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="E17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H17" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>64</v>
+        <v>195</v>
       </c>
       <c r="I17" s="2" t="n">
         <v>0</v>
@@ -1310,7 +1365,8 @@
         <v>20</v>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>172.5</v>
       </c>
       <c r="L17" s="2" t="n">
         <v>10</v>
@@ -1323,10 +1379,11 @@
       </c>
       <c r="O17" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>447.5</v>
+        <v>457.5</v>
       </c>
       <c r="P17" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>335</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1334,7 +1391,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>13</v>
@@ -1342,18 +1399,18 @@
       <c r="D18" s="4" t="n">
         <v>-83</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="E18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H18" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>103</v>
+        <v>250</v>
       </c>
       <c r="I18" s="2" t="n">
         <v>0</v>
@@ -1362,7 +1419,8 @@
         <v>20</v>
       </c>
       <c r="K18" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>217.5</v>
       </c>
       <c r="L18" s="2" t="n">
         <v>10</v>
@@ -1375,10 +1433,11 @@
       </c>
       <c r="O18" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>375</v>
+        <v>282.5</v>
       </c>
       <c r="P18" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>290</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1386,7 +1445,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>14</v>
@@ -1394,18 +1453,18 @@
       <c r="D19" s="4" t="n">
         <v>-83</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="E19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H19" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>145</v>
+        <v>177</v>
       </c>
       <c r="I19" s="2" t="n">
         <v>0</v>
@@ -1414,7 +1473,8 @@
         <v>20</v>
       </c>
       <c r="K19" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>167.5</v>
       </c>
       <c r="L19" s="2" t="n">
         <v>10</v>
@@ -1427,10 +1487,11 @@
       </c>
       <c r="O19" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>295</v>
+        <v>370</v>
       </c>
       <c r="P19" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>490</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1438,7 +1499,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>15</v>
@@ -1446,18 +1507,18 @@
       <c r="D20" s="4" t="n">
         <v>-83</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" s="1" t="s">
+      <c r="E20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H20" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>294</v>
+        <v>186</v>
       </c>
       <c r="I20" s="2" t="n">
         <v>0</v>
@@ -1466,7 +1527,8 @@
         <v>20</v>
       </c>
       <c r="K20" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>455</v>
       </c>
       <c r="L20" s="2" t="n">
         <v>10</v>
@@ -1479,10 +1541,11 @@
       </c>
       <c r="O20" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>232.5</v>
+        <v>487.5</v>
       </c>
       <c r="P20" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>427.5</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1490,7 +1553,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C21" s="4" t="n">
         <v>16</v>
@@ -1498,18 +1561,18 @@
       <c r="D21" s="4" t="n">
         <v>-83</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="E21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H21" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="I21" s="2" t="n">
         <v>0</v>
@@ -1518,7 +1581,8 @@
         <v>20</v>
       </c>
       <c r="K21" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>210</v>
       </c>
       <c r="L21" s="2" t="n">
         <v>10</v>
@@ -1531,10 +1595,11 @@
       </c>
       <c r="O21" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>182.5</v>
+        <v>220</v>
       </c>
       <c r="P21" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>297.5</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1542,7 +1607,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C22" s="4" t="n">
         <v>17</v>
@@ -1550,18 +1615,18 @@
       <c r="D22" s="4" t="n">
         <v>-83</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="E22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H22" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="I22" s="2" t="n">
         <v>0</v>
@@ -1570,7 +1635,8 @@
         <v>20</v>
       </c>
       <c r="K22" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>442.5</v>
       </c>
       <c r="L22" s="2" t="n">
         <v>10</v>
@@ -1583,10 +1649,11 @@
       </c>
       <c r="O22" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>282.5</v>
+        <v>302.5</v>
       </c>
       <c r="P22" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>475</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1594,7 +1661,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C23" s="4" t="n">
         <v>18</v>
@@ -1602,18 +1669,18 @@
       <c r="D23" s="4" t="n">
         <v>-83</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="E23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H23" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>58</v>
+        <v>181</v>
       </c>
       <c r="I23" s="2" t="n">
         <v>0</v>
@@ -1622,7 +1689,8 @@
         <v>20</v>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>110</v>
       </c>
       <c r="L23" s="2" t="n">
         <v>10</v>
@@ -1635,10 +1703,11 @@
       </c>
       <c r="O23" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>377.5</v>
+        <v>287.5</v>
       </c>
       <c r="P23" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>37.5</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1646,7 +1715,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C24" s="4" t="n">
         <v>19</v>
@@ -1654,18 +1723,18 @@
       <c r="D24" s="4" t="n">
         <v>-83</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="E24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H24" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>300</v>
+        <v>221</v>
       </c>
       <c r="I24" s="2" t="n">
         <v>0</v>
@@ -1674,7 +1743,8 @@
         <v>20</v>
       </c>
       <c r="K24" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>452.5</v>
       </c>
       <c r="L24" s="2" t="n">
         <v>10</v>
@@ -1687,10 +1757,11 @@
       </c>
       <c r="O24" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>390</v>
+        <v>420</v>
       </c>
       <c r="P24" s="2" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>457.5</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1698,7 +1769,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>24</v>
@@ -1710,14 +1781,14 @@
         <v>29</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H25" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>297</v>
+        <v>215</v>
       </c>
       <c r="I25" s="2" t="n">
         <v>10</v>
@@ -1727,7 +1798,7 @@
       </c>
       <c r="K25" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="L25" s="2" t="n">
         <v>10</v>
@@ -1740,11 +1811,11 @@
       </c>
       <c r="O25" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>462.5</v>
+        <v>57.5</v>
       </c>
       <c r="P25" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>290</v>
+        <v>292.5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1752,7 +1823,7 @@
         <v>3</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>25</v>
@@ -1764,14 +1835,14 @@
         <v>29</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>46</v>
       </c>
       <c r="H26" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="I26" s="2" t="n">
         <v>10</v>
@@ -1781,24 +1852,24 @@
       </c>
       <c r="K26" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>175</v>
+      </c>
+      <c r="L26" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="M26" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O26" s="2" t="n">
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
+        <v>260</v>
+      </c>
+      <c r="P26" s="2" t="n">
+        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
         <v>402.5</v>
-      </c>
-      <c r="L26" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="M26" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O26" s="2" t="n">
-        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>395</v>
-      </c>
-      <c r="P26" s="2" t="n">
-        <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>447.5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1806,7 +1877,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>26</v>
@@ -1818,14 +1889,14 @@
         <v>29</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H27" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>54</v>
+        <v>227</v>
       </c>
       <c r="I27" s="2" t="n">
         <v>10</v>
@@ -1835,7 +1906,7 @@
       </c>
       <c r="K27" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>310</v>
+        <v>267.5</v>
       </c>
       <c r="L27" s="2" t="n">
         <v>10</v>
@@ -1848,11 +1919,11 @@
       </c>
       <c r="O27" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>220</v>
+        <v>435</v>
       </c>
       <c r="P27" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>310</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1860,7 +1931,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>27</v>
@@ -1872,14 +1943,14 @@
         <v>29</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>41</v>
       </c>
       <c r="H28" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="I28" s="2" t="n">
         <v>10</v>
@@ -1889,7 +1960,7 @@
       </c>
       <c r="K28" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>222.5</v>
+        <v>482.5</v>
       </c>
       <c r="L28" s="2" t="n">
         <v>10</v>
@@ -1902,11 +1973,11 @@
       </c>
       <c r="O28" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>52.5</v>
+        <v>335</v>
       </c>
       <c r="P28" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>117.5</v>
+        <v>447.5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1914,7 +1985,7 @@
         <v>3</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C29" s="3" t="n">
         <v>28</v>
@@ -1926,14 +1997,14 @@
         <v>29</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H29" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="I29" s="2" t="n">
         <v>10</v>
@@ -1943,7 +2014,7 @@
       </c>
       <c r="K29" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>407.5</v>
+        <v>112.5</v>
       </c>
       <c r="L29" s="2" t="n">
         <v>10</v>
@@ -1956,11 +2027,11 @@
       </c>
       <c r="O29" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="P29" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>25</v>
+        <v>287.5</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1968,7 +2039,7 @@
         <v>3</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C30" s="3" t="n">
         <v>28</v>
@@ -1980,14 +2051,14 @@
         <v>29</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H30" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>258</v>
+        <v>152</v>
       </c>
       <c r="I30" s="2" t="n">
         <v>10</v>
@@ -1997,7 +2068,7 @@
       </c>
       <c r="K30" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>472.5</v>
+        <v>320</v>
       </c>
       <c r="L30" s="2" t="n">
         <v>10</v>
@@ -2010,11 +2081,11 @@
       </c>
       <c r="O30" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>375</v>
+        <v>85</v>
       </c>
       <c r="P30" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>285</v>
+        <v>377.5</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2022,7 +2093,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C31" s="3" t="n">
         <v>28</v>
@@ -2034,14 +2105,14 @@
         <v>29</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H31" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="I31" s="2" t="n">
         <v>10</v>
@@ -2051,7 +2122,7 @@
       </c>
       <c r="K31" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>262.5</v>
+        <v>125</v>
       </c>
       <c r="L31" s="2" t="n">
         <v>10</v>
@@ -2064,11 +2135,11 @@
       </c>
       <c r="O31" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>195</v>
+        <v>90</v>
       </c>
       <c r="P31" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>292.5</v>
+        <v>460</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2076,7 +2147,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C32" s="3" t="n">
         <v>28</v>
@@ -2088,14 +2159,14 @@
         <v>29</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H32" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>207</v>
+        <v>277</v>
       </c>
       <c r="I32" s="2" t="n">
         <v>10</v>
@@ -2105,7 +2176,7 @@
       </c>
       <c r="K32" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>450</v>
+        <v>352.5</v>
       </c>
       <c r="L32" s="2" t="n">
         <v>10</v>
@@ -2118,11 +2189,11 @@
       </c>
       <c r="O32" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>265</v>
+        <v>372.5</v>
       </c>
       <c r="P32" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>452.5</v>
+        <v>437.5</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2130,7 +2201,7 @@
         <v>3</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C33" s="3" t="n">
         <v>28</v>
@@ -2142,14 +2213,14 @@
         <v>29</v>
       </c>
       <c r="F33" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="H33" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>294</v>
+        <v>179</v>
       </c>
       <c r="I33" s="2" t="n">
         <v>10</v>
@@ -2159,7 +2230,7 @@
       </c>
       <c r="K33" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>270</v>
+        <v>400</v>
       </c>
       <c r="L33" s="2" t="n">
         <v>10</v>
@@ -2172,11 +2243,11 @@
       </c>
       <c r="O33" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>475</v>
+        <v>462.5</v>
       </c>
       <c r="P33" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>495</v>
+        <v>345</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2184,7 +2255,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C34" s="3" t="n">
         <v>28</v>
@@ -2196,14 +2267,14 @@
         <v>29</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H34" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>295</v>
+        <v>94</v>
       </c>
       <c r="I34" s="2" t="n">
         <v>10</v>
@@ -2213,7 +2284,7 @@
       </c>
       <c r="K34" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>92.5</v>
+        <v>190</v>
       </c>
       <c r="L34" s="2" t="n">
         <v>10</v>
@@ -2226,11 +2297,11 @@
       </c>
       <c r="O34" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>437.5</v>
+        <v>310</v>
       </c>
       <c r="P34" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>55</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2243,21 +2314,21 @@
       <c r="C35" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="D35" s="4" t="n">
-        <v>-83</v>
+      <c r="D35" s="2" t="n">
+        <v>-93</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H35" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>105</v>
+        <v>235</v>
       </c>
       <c r="I35" s="2" t="n">
         <v>0</v>
@@ -2279,7 +2350,7 @@
       </c>
       <c r="O35" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>380</v>
+        <v>412.5</v>
       </c>
       <c r="P35" s="2" t="n">
         <v>0</v>
@@ -2290,26 +2361,26 @@
         <v>3</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C36" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="D36" s="4" t="n">
-        <v>-83</v>
+      <c r="D36" s="2" t="n">
+        <v>-93</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F36" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H36" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>244</v>
+        <v>294</v>
       </c>
       <c r="I36" s="2" t="n">
         <v>0</v>
@@ -2331,7 +2402,7 @@
       </c>
       <c r="O36" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>47.5</v>
+        <v>400</v>
       </c>
       <c r="P36" s="2" t="n">
         <v>0</v>
@@ -2347,21 +2418,21 @@
       <c r="C37" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="D37" s="4" t="n">
-        <v>-83</v>
+      <c r="D37" s="2" t="n">
+        <v>-93</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H37" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>100</v>
+        <v>218</v>
       </c>
       <c r="I37" s="2" t="n">
         <v>0</v>
@@ -2383,7 +2454,7 @@
       </c>
       <c r="O37" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>177.5</v>
+        <v>117.5</v>
       </c>
       <c r="P37" s="2" t="n">
         <v>0</v>
@@ -2394,26 +2465,26 @@
         <v>3</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C38" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="D38" s="4" t="n">
-        <v>-83</v>
+      <c r="D38" s="2" t="n">
+        <v>-93</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H38" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>103</v>
+        <v>264</v>
       </c>
       <c r="I38" s="2" t="n">
         <v>0</v>
@@ -2435,7 +2506,7 @@
       </c>
       <c r="O38" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>480</v>
+        <v>62.5</v>
       </c>
       <c r="P38" s="2" t="n">
         <v>0</v>
@@ -2446,26 +2517,26 @@
         <v>3</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C39" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="D39" s="4" t="n">
-        <v>-83</v>
+      <c r="D39" s="2" t="n">
+        <v>-93</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F39" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H39" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>298</v>
+        <v>259</v>
       </c>
       <c r="I39" s="2" t="n">
         <v>0</v>
@@ -2487,7 +2558,7 @@
       </c>
       <c r="O39" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>375</v>
+        <v>435</v>
       </c>
       <c r="P39" s="2" t="n">
         <v>0</v>
@@ -2498,26 +2569,26 @@
         <v>3</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C40" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="D40" s="4" t="n">
-        <v>-83</v>
+      <c r="D40" s="2" t="n">
+        <v>-93</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H40" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>46</v>
+        <v>130</v>
       </c>
       <c r="I40" s="2" t="n">
         <v>0</v>
@@ -2539,7 +2610,7 @@
       </c>
       <c r="O40" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>432.5</v>
+        <v>447.5</v>
       </c>
       <c r="P40" s="2" t="n">
         <v>0</v>
@@ -2550,26 +2621,26 @@
         <v>3</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C41" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="D41" s="4" t="n">
-        <v>-83</v>
+      <c r="D41" s="2" t="n">
+        <v>-93</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H41" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="I41" s="2" t="n">
         <v>0</v>
@@ -2591,7 +2662,7 @@
       </c>
       <c r="O41" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>342.5</v>
+        <v>370</v>
       </c>
       <c r="P41" s="2" t="n">
         <v>0</v>
@@ -2602,26 +2673,26 @@
         <v>3</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C42" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="D42" s="4" t="n">
-        <v>-83</v>
+      <c r="D42" s="2" t="n">
+        <v>-93</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H42" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="I42" s="2" t="n">
         <v>0</v>
@@ -2643,7 +2714,7 @@
       </c>
       <c r="O42" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>420</v>
+        <v>180</v>
       </c>
       <c r="P42" s="2" t="n">
         <v>0</v>
@@ -2654,26 +2725,26 @@
         <v>3</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C43" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="D43" s="4" t="n">
-        <v>-83</v>
+      <c r="D43" s="2" t="n">
+        <v>-93</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H43" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="I43" s="2" t="n">
         <v>0</v>
@@ -2695,7 +2766,7 @@
       </c>
       <c r="O43" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>135</v>
+        <v>182.5</v>
       </c>
       <c r="P43" s="2" t="n">
         <v>0</v>
@@ -2706,26 +2777,26 @@
         <v>3</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C44" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="D44" s="4" t="n">
-        <v>-83</v>
+      <c r="D44" s="2" t="n">
+        <v>-93</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F44" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H44" s="2" t="n">
         <f aca="false">RANDBETWEEN(40,300)</f>
-        <v>220</v>
+        <v>70</v>
       </c>
       <c r="I44" s="2" t="n">
         <v>0</v>
@@ -2747,7 +2818,7 @@
       </c>
       <c r="O44" s="2" t="n">
         <f aca="false">RANDBETWEEN(10, 200) * 2.5</f>
-        <v>182.5</v>
+        <v>262.5</v>
       </c>
       <c r="P44" s="2" t="n">
         <v>0</v>

</xml_diff>